<commit_message>
ng: update entomo forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/april/ng_oncho_bsc_202304_1_capture.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/april/ng_oncho_bsc_202304_1_capture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\ONCHO\Breeding Site Survey\Nigeria\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\april\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65283961-D296-4C4F-A30F-A46956A9A3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFCA494-F1E5-427E-B403-E19ED0879C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="185">
   <si>
     <t>type</t>
   </si>
@@ -427,17 +425,176 @@
     <t>CHONGWOM</t>
   </si>
   <si>
-    <t>ng_oncho_bsc_202304_1_capture</t>
-  </si>
-  <si>
-    <t>(2023 April) - 1. Human Landing Catches</t>
+    <t>ng_oncho_bsc_202304_1_capture_v2_gombe</t>
+  </si>
+  <si>
+    <t>GARKO</t>
+  </si>
+  <si>
+    <t>KULANI / DEGRE /SIKKAM</t>
+  </si>
+  <si>
+    <t>MWONA</t>
+  </si>
+  <si>
+    <t>BILLIRI SOUTH</t>
+  </si>
+  <si>
+    <t>TAL</t>
+  </si>
+  <si>
+    <t>GWANI / SHINGA / WADE</t>
+  </si>
+  <si>
+    <t>JAGALI NORTH</t>
+  </si>
+  <si>
+    <t>NOEC</t>
+  </si>
+  <si>
+    <t>Modelling Sites</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>GOM_AKK_N_001</t>
+  </si>
+  <si>
+    <t>GOM_AKK_N_002</t>
+  </si>
+  <si>
+    <t>GOM_AKK_N_003</t>
+  </si>
+  <si>
+    <t>GOM_BAL_N_004</t>
+  </si>
+  <si>
+    <t>GOM_BAL_N_005</t>
+  </si>
+  <si>
+    <t>GOM_BAL_N_006</t>
+  </si>
+  <si>
+    <t>GOM_BAL_N_007</t>
+  </si>
+  <si>
+    <t>GOM_BAL_N_008</t>
+  </si>
+  <si>
+    <t>GOM_BIL_N_009</t>
+  </si>
+  <si>
+    <t>GOM_DUK_N_010</t>
+  </si>
+  <si>
+    <t>GOM_DUK_N_011</t>
+  </si>
+  <si>
+    <t>GOM_DUK_N_012</t>
+  </si>
+  <si>
+    <t>GOM_DUK_N_013</t>
+  </si>
+  <si>
+    <t>GOM_DUK_N_014</t>
+  </si>
+  <si>
+    <t>GOM_NAF_N_015</t>
+  </si>
+  <si>
+    <t>GOM_FUN_N_016</t>
+  </si>
+  <si>
+    <t>GOM_SHO_N_017</t>
+  </si>
+  <si>
+    <t>GOM_KAL_N_018</t>
+  </si>
+  <si>
+    <t>GOM_KWA_N_019</t>
+  </si>
+  <si>
+    <t>GOM_NAF_N_020</t>
+  </si>
+  <si>
+    <t>GOM_NAF_N_021</t>
+  </si>
+  <si>
+    <t>GOM_NAF_N_022</t>
+  </si>
+  <si>
+    <t>GOM_NAF_N_023</t>
+  </si>
+  <si>
+    <t>GOM_NAF_N_024</t>
+  </si>
+  <si>
+    <t>GOM_SHO_N_025</t>
+  </si>
+  <si>
+    <t>GOM_YAL_N_026</t>
+  </si>
+  <si>
+    <t>GOM_SHO_N_027</t>
+  </si>
+  <si>
+    <t>GOM_AKK_M_028</t>
+  </si>
+  <si>
+    <t>GOM_AKK_M_029</t>
+  </si>
+  <si>
+    <t>GOM_AKK_M_030</t>
+  </si>
+  <si>
+    <t>GOM_BAL_M_031</t>
+  </si>
+  <si>
+    <t>GOM_BAL_M_032</t>
+  </si>
+  <si>
+    <t>GOM_BIL_M_033</t>
+  </si>
+  <si>
+    <t>GOM_BIL_M_034</t>
+  </si>
+  <si>
+    <t>GOM_BIL_M_035</t>
+  </si>
+  <si>
+    <t>GOM_YAM_M_036</t>
+  </si>
+  <si>
+    <t>GOM_YAM_M_037</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>select_one site</t>
+  </si>
+  <si>
+    <t>select_one site_id</t>
+  </si>
+  <si>
+    <t>community = ${s_community}</t>
+  </si>
+  <si>
+    <t>allow_choice_duplicates</t>
+  </si>
+  <si>
+    <t>site = ${s_site}</t>
+  </si>
+  <si>
+    <t>(2023 July) - 1. Gombe state - Human Landing Catches V2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -476,6 +633,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -539,12 +704,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -579,6 +741,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -865,11 +1035,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -885,461 +1055,465 @@
     <col min="9" max="9" width="12.625" customWidth="1"/>
     <col min="10" max="10" width="9.75" customWidth="1"/>
     <col min="11" max="11" width="13.875" customWidth="1"/>
-    <col min="12" max="12" width="39.625" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="37.5">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="37.5">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1">
+    <row r="2" spans="1:13" s="2" customFormat="1">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1">
-      <c r="A3" s="9" t="s">
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="9" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:13" s="2" customFormat="1">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="9" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:13" s="2" customFormat="1">
+      <c r="A5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="21" customHeight="1">
+      <c r="A6" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1">
+      <c r="A7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1">
+      <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1">
+      <c r="A11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1">
-      <c r="A7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6" t="s">
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1">
+      <c r="A12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1">
+      <c r="A13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1">
+      <c r="A14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1">
+      <c r="A15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="H15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1">
+      <c r="A16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1">
+      <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1">
-      <c r="A9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1">
-      <c r="A10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1">
-      <c r="A11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1">
-      <c r="A12" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1">
-      <c r="A13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1">
-      <c r="A14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="H14" s="9" t="s">
+      <c r="B17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="H17" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" s="3" customFormat="1">
-      <c r="A15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1">
-      <c r="A16" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="1:12" s="3" customFormat="1">
-      <c r="A17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-    </row>
-    <row r="18" spans="1:12" s="3" customFormat="1">
-      <c r="A18" s="6" t="s">
+      <c r="I17" s="8"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1">
+      <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" s="3" customFormat="1">
-      <c r="A19" s="9" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1">
+      <c r="A19" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-    </row>
-    <row r="20" spans="1:12" s="3" customFormat="1">
-      <c r="A20" s="9" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1">
+      <c r="A20" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="1:12" s="3" customFormat="1">
-      <c r="B21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" s="2" customFormat="1">
+      <c r="B21" s="13"/>
+      <c r="D21" s="13"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:12" s="3" customFormat="1">
-      <c r="B22" s="14"/>
-      <c r="D22" s="14"/>
+    <row r="22" spans="1:12" s="2" customFormat="1">
+      <c r="B22" s="13"/>
+      <c r="D22" s="13"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:12" s="3" customFormat="1">
+    <row r="23" spans="1:12" s="2" customFormat="1">
       <c r="B23"/>
       <c r="D23"/>
       <c r="G23"/>
@@ -1352,11 +1526,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD59"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1366,29 +1540,33 @@
     <col min="3" max="3" width="23.125" customWidth="1"/>
     <col min="4" max="4" width="13.125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1399,7 +1577,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1410,7 +1588,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1421,7 +1599,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1432,7 +1610,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1443,7 +1621,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1454,7 +1632,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1465,7 +1643,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1476,7 +1654,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1487,7 +1665,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1498,7 +1676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1509,33 +1687,33 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="6" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1546,7 +1724,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -1600,7 +1778,7 @@
       <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1614,7 +1792,7 @@
       <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1628,7 +1806,7 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1642,7 +1820,7 @@
       <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1656,7 +1834,7 @@
       <c r="C26" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1670,7 +1848,7 @@
       <c r="C27" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1684,7 +1862,7 @@
       <c r="C28" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1698,7 +1876,7 @@
       <c r="C29" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1712,7 +1890,7 @@
       <c r="C30" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1726,7 +1904,7 @@
       <c r="C31" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1735,10 +1913,10 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
         <v>95</v>
@@ -1749,10 +1927,10 @@
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E34" t="s">
         <v>95</v>
@@ -1763,10 +1941,10 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="E35" t="s">
         <v>95</v>
@@ -1777,13 +1955,13 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1791,13 +1969,13 @@
         <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1805,13 +1983,13 @@
         <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1819,10 +1997,10 @@
         <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
         <v>96</v>
@@ -1833,10 +2011,10 @@
         <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E40" t="s">
         <v>96</v>
@@ -1847,13 +2025,13 @@
         <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1861,13 +2039,13 @@
         <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1875,13 +2053,13 @@
         <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1889,13 +2067,13 @@
         <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1903,13 +2081,13 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1917,13 +2095,13 @@
         <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1931,13 +2109,13 @@
         <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1945,13 +2123,13 @@
         <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1959,13 +2137,13 @@
         <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1973,13 +2151,13 @@
         <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1987,13 +2165,13 @@
         <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2001,13 +2179,13 @@
         <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2015,13 +2193,13 @@
         <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2029,13 +2207,13 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E54" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2043,13 +2221,13 @@
         <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2057,13 +2235,13 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2071,13 +2249,13 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2085,13 +2263,13 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C58" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2099,13 +2277,1175 @@
         <v>70</v>
       </c>
       <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" t="s">
+        <v>99</v>
+      </c>
+      <c r="E62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+      <c r="E66" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
         <v>128</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C67" t="s">
         <v>128</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E67" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" t="s">
+        <v>137</v>
+      </c>
+      <c r="E68" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" t="s">
+        <v>138</v>
+      </c>
+      <c r="F70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" t="s">
+        <v>138</v>
+      </c>
+      <c r="F71" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" t="s">
+        <v>138</v>
+      </c>
+      <c r="F73" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" t="s">
+        <v>138</v>
+      </c>
+      <c r="F74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" t="s">
+        <v>138</v>
+      </c>
+      <c r="F75" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" t="s">
+        <v>138</v>
+      </c>
+      <c r="F76" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" t="s">
+        <v>138</v>
+      </c>
+      <c r="F77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B78" t="s">
+        <v>138</v>
+      </c>
+      <c r="C78" t="s">
+        <v>138</v>
+      </c>
+      <c r="F78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" t="s">
+        <v>138</v>
+      </c>
+      <c r="F79" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" t="s">
+        <v>138</v>
+      </c>
+      <c r="F80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" t="s">
+        <v>138</v>
+      </c>
+      <c r="F81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" t="s">
+        <v>138</v>
+      </c>
+      <c r="F82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
+        <v>138</v>
+      </c>
+      <c r="C83" t="s">
+        <v>138</v>
+      </c>
+      <c r="F83" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" t="s">
+        <v>138</v>
+      </c>
+      <c r="F84" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" t="s">
+        <v>138</v>
+      </c>
+      <c r="F85" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B86" t="s">
+        <v>138</v>
+      </c>
+      <c r="C86" t="s">
+        <v>138</v>
+      </c>
+      <c r="F86" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" t="s">
+        <v>138</v>
+      </c>
+      <c r="C87" t="s">
+        <v>138</v>
+      </c>
+      <c r="F87" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" t="s">
+        <v>138</v>
+      </c>
+      <c r="C88" t="s">
+        <v>138</v>
+      </c>
+      <c r="F88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" t="s">
+        <v>138</v>
+      </c>
+      <c r="F89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" t="s">
+        <v>138</v>
+      </c>
+      <c r="C90" t="s">
+        <v>138</v>
+      </c>
+      <c r="F90" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" t="s">
+        <v>138</v>
+      </c>
+      <c r="F91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" t="s">
+        <v>138</v>
+      </c>
+      <c r="C92" t="s">
+        <v>138</v>
+      </c>
+      <c r="F92" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" t="s">
+        <v>138</v>
+      </c>
+      <c r="C93" t="s">
+        <v>138</v>
+      </c>
+      <c r="F93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B94" t="s">
+        <v>138</v>
+      </c>
+      <c r="C94" t="s">
+        <v>138</v>
+      </c>
+      <c r="F94" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95" t="s">
+        <v>138</v>
+      </c>
+      <c r="F95" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B96" t="s">
+        <v>138</v>
+      </c>
+      <c r="C96" t="s">
+        <v>138</v>
+      </c>
+      <c r="F96" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" t="s">
+        <v>139</v>
+      </c>
+      <c r="C97" t="s">
+        <v>139</v>
+      </c>
+      <c r="F97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B98" t="s">
+        <v>139</v>
+      </c>
+      <c r="C98" t="s">
+        <v>139</v>
+      </c>
+      <c r="F98" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B99" t="s">
+        <v>139</v>
+      </c>
+      <c r="C99" t="s">
+        <v>139</v>
+      </c>
+      <c r="F99" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B100" t="s">
+        <v>139</v>
+      </c>
+      <c r="C100" t="s">
+        <v>139</v>
+      </c>
+      <c r="F100" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B101" t="s">
+        <v>139</v>
+      </c>
+      <c r="C101" t="s">
+        <v>139</v>
+      </c>
+      <c r="F101" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B102" t="s">
+        <v>139</v>
+      </c>
+      <c r="C102" t="s">
+        <v>139</v>
+      </c>
+      <c r="F102" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B103" t="s">
+        <v>139</v>
+      </c>
+      <c r="C103" t="s">
+        <v>139</v>
+      </c>
+      <c r="F103" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" t="s">
+        <v>139</v>
+      </c>
+      <c r="C104" t="s">
+        <v>139</v>
+      </c>
+      <c r="F104" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B105" t="s">
+        <v>139</v>
+      </c>
+      <c r="C105" t="s">
+        <v>139</v>
+      </c>
+      <c r="F105" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B106" t="s">
+        <v>139</v>
+      </c>
+      <c r="C106" t="s">
+        <v>139</v>
+      </c>
+      <c r="F106" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B108" t="s">
+        <v>141</v>
+      </c>
+      <c r="C108" t="s">
+        <v>141</v>
+      </c>
+      <c r="G108" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B109" t="s">
+        <v>142</v>
+      </c>
+      <c r="C109" t="s">
+        <v>142</v>
+      </c>
+      <c r="G109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B110" t="s">
+        <v>143</v>
+      </c>
+      <c r="C110" t="s">
+        <v>143</v>
+      </c>
+      <c r="G110" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B111" t="s">
+        <v>144</v>
+      </c>
+      <c r="C111" t="s">
+        <v>144</v>
+      </c>
+      <c r="G111" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" t="s">
+        <v>145</v>
+      </c>
+      <c r="C112" t="s">
+        <v>145</v>
+      </c>
+      <c r="G112" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B113" t="s">
+        <v>146</v>
+      </c>
+      <c r="C113" t="s">
+        <v>146</v>
+      </c>
+      <c r="G113" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B114" t="s">
+        <v>147</v>
+      </c>
+      <c r="C114" t="s">
+        <v>147</v>
+      </c>
+      <c r="G114" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115" t="s">
+        <v>148</v>
+      </c>
+      <c r="C115" t="s">
+        <v>148</v>
+      </c>
+      <c r="G115" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B116" t="s">
+        <v>149</v>
+      </c>
+      <c r="C116" t="s">
+        <v>149</v>
+      </c>
+      <c r="G116" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B117" t="s">
+        <v>150</v>
+      </c>
+      <c r="C117" t="s">
+        <v>150</v>
+      </c>
+      <c r="G117" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B118" t="s">
+        <v>151</v>
+      </c>
+      <c r="C118" t="s">
+        <v>151</v>
+      </c>
+      <c r="G118" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B119" t="s">
+        <v>152</v>
+      </c>
+      <c r="C119" t="s">
+        <v>152</v>
+      </c>
+      <c r="G119" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B120" t="s">
+        <v>153</v>
+      </c>
+      <c r="C120" t="s">
+        <v>153</v>
+      </c>
+      <c r="G120" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B121" t="s">
+        <v>154</v>
+      </c>
+      <c r="C121" t="s">
+        <v>154</v>
+      </c>
+      <c r="G121" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B122" t="s">
+        <v>155</v>
+      </c>
+      <c r="C122" t="s">
+        <v>155</v>
+      </c>
+      <c r="G122" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B123" t="s">
+        <v>156</v>
+      </c>
+      <c r="C123" t="s">
+        <v>156</v>
+      </c>
+      <c r="G123" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B124" t="s">
+        <v>157</v>
+      </c>
+      <c r="C124" t="s">
+        <v>157</v>
+      </c>
+      <c r="G124" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B125" t="s">
+        <v>158</v>
+      </c>
+      <c r="C125" t="s">
+        <v>158</v>
+      </c>
+      <c r="G125" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B126" t="s">
+        <v>159</v>
+      </c>
+      <c r="C126" t="s">
+        <v>159</v>
+      </c>
+      <c r="G126" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B127" t="s">
+        <v>160</v>
+      </c>
+      <c r="C127" t="s">
+        <v>160</v>
+      </c>
+      <c r="G127" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B128" t="s">
+        <v>161</v>
+      </c>
+      <c r="C128" t="s">
+        <v>161</v>
+      </c>
+      <c r="G128" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B129" t="s">
+        <v>162</v>
+      </c>
+      <c r="C129" t="s">
+        <v>162</v>
+      </c>
+      <c r="G129" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B130" t="s">
+        <v>163</v>
+      </c>
+      <c r="C130" t="s">
+        <v>163</v>
+      </c>
+      <c r="G130" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B131" t="s">
+        <v>164</v>
+      </c>
+      <c r="C131" t="s">
+        <v>164</v>
+      </c>
+      <c r="G131" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B132" t="s">
+        <v>165</v>
+      </c>
+      <c r="C132" t="s">
+        <v>165</v>
+      </c>
+      <c r="G132" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B133" t="s">
+        <v>166</v>
+      </c>
+      <c r="C133" t="s">
+        <v>166</v>
+      </c>
+      <c r="G133" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B134" t="s">
+        <v>167</v>
+      </c>
+      <c r="C134" t="s">
+        <v>167</v>
+      </c>
+      <c r="G134" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B135" t="s">
+        <v>168</v>
+      </c>
+      <c r="C135" t="s">
+        <v>168</v>
+      </c>
+      <c r="G135" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B136" t="s">
+        <v>169</v>
+      </c>
+      <c r="C136" t="s">
+        <v>169</v>
+      </c>
+      <c r="G136" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B137" t="s">
+        <v>170</v>
+      </c>
+      <c r="C137" t="s">
+        <v>170</v>
+      </c>
+      <c r="G137" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B138" t="s">
+        <v>171</v>
+      </c>
+      <c r="C138" t="s">
+        <v>171</v>
+      </c>
+      <c r="G138" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B139" t="s">
+        <v>172</v>
+      </c>
+      <c r="C139" t="s">
+        <v>172</v>
+      </c>
+      <c r="G139" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B140" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" t="s">
+        <v>173</v>
+      </c>
+      <c r="G140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B141" t="s">
+        <v>174</v>
+      </c>
+      <c r="C141" t="s">
+        <v>174</v>
+      </c>
+      <c r="G141" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B142" t="s">
+        <v>175</v>
+      </c>
+      <c r="C142" t="s">
+        <v>175</v>
+      </c>
+      <c r="G142" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B143" t="s">
+        <v>176</v>
+      </c>
+      <c r="C143" t="s">
+        <v>176</v>
+      </c>
+      <c r="G143" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B144" t="s">
+        <v>177</v>
+      </c>
+      <c r="C144" t="s">
+        <v>177</v>
+      </c>
+      <c r="G144" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2119,45 +3459,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="44.125" customWidth="1"/>
-    <col min="2" max="2" width="34.75" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="44.125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="34.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="20">
         <v>20210625</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="20" t="s">
         <v>93</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>